<commit_message>
new changes dated 18th Dec
</commit_message>
<xml_diff>
--- a/data/input/Data-Input.xlsx
+++ b/data/input/Data-Input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe0e69aeb448a87c/Documents/Chandrika/Makers Lab/AI Based Deal Win Probability/POC - Probability Tool/data/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe0e69aeb448a87c/Documents/Chandrika/Makers Lab/AI Based Deal Win Probability/POC- Probability Tool -Git/POC-Probability-Tool/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{A73F2F1E-D1CB-4D13-997B-6C51AE4AA993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A577A9BC-C7D7-43B1-9765-3281B84666C0}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{A73F2F1E-D1CB-4D13-997B-6C51AE4AA993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59287655-1F2F-4445-8B7D-EA06AD8E86D1}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="Template" sheetId="13" r:id="rId1"/>
     <sheet name="SST Involved WLA_02.07.24" sheetId="4" state="hidden" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Template!#REF!</definedName>
     <definedName name="Capability_or_Credentials">#REF!</definedName>
@@ -43,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="285">
   <si>
     <t>CRM ID</t>
   </si>
@@ -870,18 +873,6 @@
     <t>Type of Business</t>
   </si>
   <si>
-    <t>Etihad</t>
-  </si>
-  <si>
-    <t>Opportunity 1</t>
-  </si>
-  <si>
-    <t>Q2'25</t>
-  </si>
-  <si>
-    <t>EN</t>
-  </si>
-  <si>
     <t>Qtr of closure</t>
   </si>
   <si>
@@ -921,13 +912,37 @@
     <t>BM</t>
   </si>
   <si>
-    <t>CRM300564</t>
-  </si>
-  <si>
-    <t>US</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Q4'24</t>
+  </si>
+  <si>
+    <t>Verizon</t>
+  </si>
+  <si>
+    <t>VCG VZI Visible Operations</t>
+  </si>
+  <si>
+    <t>Relationship</t>
+  </si>
+  <si>
+    <t>Quality 360° Deal Intelligence/Validation (incl win price)</t>
+  </si>
+  <si>
+    <t>Client Relationship (CXOs, decision makers, influencers)</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>Technical Response Quality (coherent, competitive, consultative, competitive)</t>
+  </si>
+  <si>
+    <t>Clear upfront understanding of what will help us win, strong customer connect and relationship building, continuous in-person engagement with the customer helped us understand their needs and requirements, intelligence about target price, ability to address all customer requirements</t>
+  </si>
+  <si>
+    <t>Sudarshan Chacko</t>
   </si>
 </sst>
 </file>
@@ -940,7 +955,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1035,8 +1050,21 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1073,8 +1101,13 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1152,16 +1185,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1262,11 +1309,39 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Comma 2" xfId="3" xr:uid="{927F8994-2CD4-4A2D-8F73-FC2384C1AF24}"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Currency 2" xfId="4" xr:uid="{F0F95EE8-F28E-4753-8CE9-EB9F90F35891}"/>
+    <cellStyle name="Good" xfId="6" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="5" xr:uid="{CDADD67D-9D84-460B-9EAE-EAB4EBC46517}"/>
@@ -1435,6 +1510,1405 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="FY25 Pipeline"/>
+      <sheetName val="Pipeline ageing"/>
+      <sheetName val="ADMS V1"/>
+      <sheetName val="Pivot"/>
+      <sheetName val="ADMS"/>
+      <sheetName val="Pivot (2)"/>
+      <sheetName val="Proactive Deals"/>
+      <sheetName val="EMEA_Table"/>
+      <sheetName val="Transition Tracker"/>
+      <sheetName val="Transition - Tracker"/>
+      <sheetName val="Deal Allocation Tracker"/>
+      <sheetName val="FY24 WLA"/>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Overview"/>
+      <sheetName val="QoQ"/>
+      <sheetName val="IBG gr"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>CRM ID</v>
+          </cell>
+          <cell r="AD1" t="str">
+            <v>Type of Business</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>263919</v>
+          </cell>
+          <cell r="AD2" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>243607</v>
+          </cell>
+          <cell r="AD3" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>290509</v>
+          </cell>
+          <cell r="AD4" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>264787</v>
+          </cell>
+          <cell r="AD5" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>256394</v>
+          </cell>
+          <cell r="AD6" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>270551</v>
+          </cell>
+          <cell r="AD7" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>265724</v>
+          </cell>
+          <cell r="AD8" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>218995</v>
+          </cell>
+          <cell r="AD9" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>257780</v>
+          </cell>
+          <cell r="AD10" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>250273</v>
+          </cell>
+          <cell r="AD11" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>245875</v>
+          </cell>
+          <cell r="AD12" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>298935</v>
+          </cell>
+          <cell r="AD13" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>294569</v>
+          </cell>
+          <cell r="AD14" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>243049</v>
+          </cell>
+          <cell r="AD15" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16">
+            <v>246355</v>
+          </cell>
+          <cell r="AD16" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17">
+            <v>261294</v>
+          </cell>
+          <cell r="AD17" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>295218</v>
+          </cell>
+          <cell r="AD18" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>248998</v>
+          </cell>
+          <cell r="AD19" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>248616</v>
+          </cell>
+          <cell r="AD20" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>263907</v>
+          </cell>
+          <cell r="AD21" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>277502</v>
+          </cell>
+          <cell r="AD22" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23">
+            <v>259278</v>
+          </cell>
+          <cell r="AD23" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24">
+            <v>281912</v>
+          </cell>
+          <cell r="AD24" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25">
+            <v>287922</v>
+          </cell>
+          <cell r="AD25" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26">
+            <v>275515</v>
+          </cell>
+          <cell r="AD26" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27">
+            <v>258888</v>
+          </cell>
+          <cell r="AD27" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28">
+            <v>290302</v>
+          </cell>
+          <cell r="AD28" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29">
+            <v>199713</v>
+          </cell>
+          <cell r="AD29" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30">
+            <v>193677</v>
+          </cell>
+          <cell r="AD30" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31">
+            <v>258557</v>
+          </cell>
+          <cell r="AD31" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32">
+            <v>292205</v>
+          </cell>
+          <cell r="AD32" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33">
+            <v>291711</v>
+          </cell>
+          <cell r="AD33" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34">
+            <v>248520</v>
+          </cell>
+          <cell r="AD34" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35">
+            <v>259256</v>
+          </cell>
+          <cell r="AD35" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36">
+            <v>238491</v>
+          </cell>
+          <cell r="AD36" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37">
+            <v>302940</v>
+          </cell>
+          <cell r="AD37" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38">
+            <v>214766</v>
+          </cell>
+          <cell r="AD38" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39">
+            <v>262750</v>
+          </cell>
+          <cell r="AD39" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40">
+            <v>273726</v>
+          </cell>
+          <cell r="AD40" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41">
+            <v>269568</v>
+          </cell>
+          <cell r="AD41" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42">
+            <v>225058</v>
+          </cell>
+          <cell r="AD42" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43">
+            <v>263767</v>
+          </cell>
+          <cell r="AD43" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44">
+            <v>230871</v>
+          </cell>
+          <cell r="AD44" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45">
+            <v>133706</v>
+          </cell>
+          <cell r="AD45" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46">
+            <v>273931</v>
+          </cell>
+          <cell r="AD46" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47">
+            <v>265721</v>
+          </cell>
+          <cell r="AD47" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48">
+            <v>241345</v>
+          </cell>
+          <cell r="AD48" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49">
+            <v>250184</v>
+          </cell>
+          <cell r="AD49" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50">
+            <v>258889</v>
+          </cell>
+          <cell r="AD50" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51">
+            <v>270396</v>
+          </cell>
+          <cell r="AD51" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52">
+            <v>269665</v>
+          </cell>
+          <cell r="AD52" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="A53">
+            <v>276645</v>
+          </cell>
+          <cell r="AD53" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="A54">
+            <v>270135</v>
+          </cell>
+          <cell r="AD54" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="A55">
+            <v>294814</v>
+          </cell>
+          <cell r="AD55" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="A56">
+            <v>218886</v>
+          </cell>
+          <cell r="AD56" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="A57">
+            <v>250413</v>
+          </cell>
+          <cell r="AD57" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="A58">
+            <v>270829</v>
+          </cell>
+          <cell r="AD58" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="A59">
+            <v>267502</v>
+          </cell>
+          <cell r="AD59" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="A60">
+            <v>273033</v>
+          </cell>
+          <cell r="AD60" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="A61">
+            <v>225357</v>
+          </cell>
+          <cell r="AD61" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="A62">
+            <v>262877</v>
+          </cell>
+          <cell r="AD62" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="A63">
+            <v>230835</v>
+          </cell>
+          <cell r="AD63" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="A64">
+            <v>247034</v>
+          </cell>
+          <cell r="AD64" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="A65">
+            <v>269958</v>
+          </cell>
+          <cell r="AD65" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="A66">
+            <v>269268</v>
+          </cell>
+          <cell r="AD66" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="A67">
+            <v>259800</v>
+          </cell>
+          <cell r="AD67" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="A68">
+            <v>288119</v>
+          </cell>
+          <cell r="AD68" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="A69">
+            <v>270733</v>
+          </cell>
+          <cell r="AD69" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="A70">
+            <v>274290</v>
+          </cell>
+          <cell r="AD70" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="A71">
+            <v>256152</v>
+          </cell>
+          <cell r="AD71" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="A72">
+            <v>237285</v>
+          </cell>
+          <cell r="AD72" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="A73">
+            <v>243703</v>
+          </cell>
+          <cell r="AD73" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="A74">
+            <v>237223</v>
+          </cell>
+          <cell r="AD74" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="A75">
+            <v>219327</v>
+          </cell>
+          <cell r="AD75" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="A76">
+            <v>111832</v>
+          </cell>
+          <cell r="AD76" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="A77">
+            <v>259291</v>
+          </cell>
+          <cell r="AD77" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="A78" t="str">
+            <v>Unknown</v>
+          </cell>
+          <cell r="AD78" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="A79">
+            <v>260129</v>
+          </cell>
+          <cell r="AD79" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="A80">
+            <v>260585</v>
+          </cell>
+          <cell r="AD80" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="A81">
+            <v>273209</v>
+          </cell>
+          <cell r="AD81" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="A82">
+            <v>267645</v>
+          </cell>
+          <cell r="AD82" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="A83">
+            <v>261223</v>
+          </cell>
+          <cell r="AD83" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="A84">
+            <v>270366</v>
+          </cell>
+          <cell r="AD84" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="A85">
+            <v>243632</v>
+          </cell>
+          <cell r="AD85" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="86">
+          <cell r="A86">
+            <v>247324</v>
+          </cell>
+          <cell r="AD86" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="87">
+          <cell r="A87">
+            <v>269990</v>
+          </cell>
+          <cell r="AD87" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="88">
+          <cell r="A88">
+            <v>269261</v>
+          </cell>
+          <cell r="AD88" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="89">
+          <cell r="A89">
+            <v>244259</v>
+          </cell>
+          <cell r="AD89" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="90">
+          <cell r="A90">
+            <v>265975</v>
+          </cell>
+          <cell r="AD90" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="91">
+          <cell r="A91">
+            <v>270851</v>
+          </cell>
+          <cell r="AD91" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="92">
+          <cell r="A92">
+            <v>236964</v>
+          </cell>
+          <cell r="AD92" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="93">
+          <cell r="A93">
+            <v>267483</v>
+          </cell>
+          <cell r="AD93" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="94">
+          <cell r="A94">
+            <v>168609</v>
+          </cell>
+          <cell r="AD94" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="95">
+          <cell r="A95">
+            <v>222536</v>
+          </cell>
+          <cell r="AD95" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="96">
+          <cell r="A96">
+            <v>245950</v>
+          </cell>
+          <cell r="AD96" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="97">
+          <cell r="A97">
+            <v>275080</v>
+          </cell>
+          <cell r="AD97" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="98">
+          <cell r="A98">
+            <v>247895</v>
+          </cell>
+          <cell r="AD98" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="99">
+          <cell r="A99">
+            <v>215045</v>
+          </cell>
+          <cell r="AD99" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="100">
+          <cell r="A100">
+            <v>217694</v>
+          </cell>
+          <cell r="AD100" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="A101">
+            <v>270827</v>
+          </cell>
+          <cell r="AD101" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="102">
+          <cell r="A102">
+            <v>255839</v>
+          </cell>
+          <cell r="AD102" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="103">
+          <cell r="A103">
+            <v>248543</v>
+          </cell>
+          <cell r="AD103" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="104">
+          <cell r="A104">
+            <v>267387</v>
+          </cell>
+          <cell r="AD104" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="105">
+          <cell r="A105">
+            <v>274860</v>
+          </cell>
+          <cell r="AD105" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="106">
+          <cell r="A106">
+            <v>243374</v>
+          </cell>
+          <cell r="AD106" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="107">
+          <cell r="A107">
+            <v>269870</v>
+          </cell>
+          <cell r="AD107" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="108">
+          <cell r="A108">
+            <v>255708</v>
+          </cell>
+          <cell r="AD108" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="109">
+          <cell r="A109">
+            <v>195774</v>
+          </cell>
+          <cell r="AD109" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="110">
+          <cell r="A110">
+            <v>204458</v>
+          </cell>
+          <cell r="AD110" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="111">
+          <cell r="A111">
+            <v>262524</v>
+          </cell>
+          <cell r="AD111" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="112">
+          <cell r="A112">
+            <v>259054</v>
+          </cell>
+          <cell r="AD112" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="113">
+          <cell r="A113">
+            <v>269049</v>
+          </cell>
+          <cell r="AD113" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="114">
+          <cell r="A114">
+            <v>273609</v>
+          </cell>
+          <cell r="AD114" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="115">
+          <cell r="A115">
+            <v>296625</v>
+          </cell>
+          <cell r="AD115" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="116">
+          <cell r="A116">
+            <v>265784</v>
+          </cell>
+          <cell r="AD116" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="117">
+          <cell r="A117">
+            <v>247327</v>
+          </cell>
+          <cell r="AD117" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="118">
+          <cell r="A118">
+            <v>237004</v>
+          </cell>
+          <cell r="AD118" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="119">
+          <cell r="A119">
+            <v>263486</v>
+          </cell>
+          <cell r="AD119" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="120">
+          <cell r="A120">
+            <v>261058</v>
+          </cell>
+          <cell r="AD120" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="121">
+          <cell r="A121">
+            <v>264631</v>
+          </cell>
+          <cell r="AD121" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="122">
+          <cell r="A122">
+            <v>293344</v>
+          </cell>
+          <cell r="AD122" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="123">
+          <cell r="A123">
+            <v>273781</v>
+          </cell>
+          <cell r="AD123" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="124">
+          <cell r="A124">
+            <v>260473</v>
+          </cell>
+          <cell r="AD124" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="125">
+          <cell r="A125">
+            <v>244015</v>
+          </cell>
+          <cell r="AD125" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="126">
+          <cell r="A126">
+            <v>253350</v>
+          </cell>
+          <cell r="AD126" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="127">
+          <cell r="A127">
+            <v>260935</v>
+          </cell>
+          <cell r="AD127" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="128">
+          <cell r="A128">
+            <v>216362</v>
+          </cell>
+          <cell r="AD128" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="129">
+          <cell r="A129">
+            <v>226727</v>
+          </cell>
+          <cell r="AD129" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="130">
+          <cell r="A130">
+            <v>214534</v>
+          </cell>
+          <cell r="AD130" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="131">
+          <cell r="A131">
+            <v>264579</v>
+          </cell>
+          <cell r="AD131" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="132">
+          <cell r="A132">
+            <v>276560</v>
+          </cell>
+          <cell r="AD132" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="133">
+          <cell r="A133">
+            <v>258134</v>
+          </cell>
+          <cell r="AD133" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="134">
+          <cell r="A134">
+            <v>269064</v>
+          </cell>
+          <cell r="AD134" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="135">
+          <cell r="A135">
+            <v>294423</v>
+          </cell>
+          <cell r="AD135" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="136">
+          <cell r="A136">
+            <v>245650</v>
+          </cell>
+          <cell r="AD136" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="137">
+          <cell r="A137">
+            <v>271600</v>
+          </cell>
+          <cell r="AD137" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="138">
+          <cell r="A138">
+            <v>274334</v>
+          </cell>
+          <cell r="AD138" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="139">
+          <cell r="A139">
+            <v>244017</v>
+          </cell>
+          <cell r="AD139" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="140">
+          <cell r="A140">
+            <v>263379</v>
+          </cell>
+          <cell r="AD140" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="141">
+          <cell r="A141">
+            <v>218945</v>
+          </cell>
+          <cell r="AD141" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="142">
+          <cell r="A142">
+            <v>259236</v>
+          </cell>
+          <cell r="AD142" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="143">
+          <cell r="A143">
+            <v>245127</v>
+          </cell>
+          <cell r="AD143" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="144">
+          <cell r="A144">
+            <v>227268</v>
+          </cell>
+          <cell r="AD144" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="145">
+          <cell r="A145">
+            <v>181145</v>
+          </cell>
+          <cell r="AD145" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="146">
+          <cell r="A146">
+            <v>241337</v>
+          </cell>
+          <cell r="AD146" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="147">
+          <cell r="A147">
+            <v>291630</v>
+          </cell>
+          <cell r="AD147" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="148">
+          <cell r="A148">
+            <v>238533</v>
+          </cell>
+          <cell r="AD148" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="149">
+          <cell r="A149">
+            <v>247993</v>
+          </cell>
+          <cell r="AD149" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="150">
+          <cell r="A150">
+            <v>260768</v>
+          </cell>
+          <cell r="AD150" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="151">
+          <cell r="A151">
+            <v>228144</v>
+          </cell>
+          <cell r="AD151" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="152">
+          <cell r="A152">
+            <v>274187</v>
+          </cell>
+          <cell r="AD152" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="153">
+          <cell r="A153">
+            <v>192073</v>
+          </cell>
+          <cell r="AD153" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="154">
+          <cell r="A154">
+            <v>236880</v>
+          </cell>
+          <cell r="AD154" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="155">
+          <cell r="A155">
+            <v>258156</v>
+          </cell>
+          <cell r="AD155" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="156">
+          <cell r="A156">
+            <v>263864</v>
+          </cell>
+          <cell r="AD156" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="157">
+          <cell r="A157">
+            <v>246200</v>
+          </cell>
+          <cell r="AD157" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="158">
+          <cell r="A158">
+            <v>276617</v>
+          </cell>
+          <cell r="AD158" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="159">
+          <cell r="A159">
+            <v>271490</v>
+          </cell>
+          <cell r="AD159" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="160">
+          <cell r="A160">
+            <v>260008</v>
+          </cell>
+          <cell r="AD160" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="161">
+          <cell r="A161">
+            <v>258807</v>
+          </cell>
+          <cell r="AD161" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="162">
+          <cell r="A162">
+            <v>214695</v>
+          </cell>
+          <cell r="AD162" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="163">
+          <cell r="A163">
+            <v>260817</v>
+          </cell>
+          <cell r="AD163" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="164">
+          <cell r="A164">
+            <v>264860</v>
+          </cell>
+          <cell r="AD164" t="str">
+            <v>NN</v>
+          </cell>
+        </row>
+        <row r="165">
+          <cell r="A165">
+            <v>246490</v>
+          </cell>
+          <cell r="AD165" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="166">
+          <cell r="A166">
+            <v>271483</v>
+          </cell>
+          <cell r="AD166" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="167">
+          <cell r="A167">
+            <v>273678</v>
+          </cell>
+          <cell r="AD167" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="168">
+          <cell r="A168">
+            <v>236408</v>
+          </cell>
+          <cell r="AD168" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+        <row r="169">
+          <cell r="A169" t="str">
+            <v>-</v>
+          </cell>
+          <cell r="AD169" t="str">
+            <v>EN</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/namedSheetViews/namedSheetView1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1708,12 +3182,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB57C08-DBA7-4474-81D3-5BFCB29EBB39}">
-  <dimension ref="A2:AF3"/>
+  <dimension ref="A2:AD3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="S2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Q2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="AF3" sqref="AF3"/>
+      <selection pane="bottomLeft" activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1726,24 +3200,23 @@
     <col min="6" max="6" width="17.26953125" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.7265625" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="18.7265625" style="8" customWidth="1"/>
-    <col min="11" max="11" width="15.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.453125" style="25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.6328125" style="25" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="71.7265625" style="25" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.453125" style="25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.6328125" style="25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="71.7265625" style="25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.08984375" style="25" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.1796875" style="1"/>
     <col min="20" max="20" width="9.1796875" style="25"/>
     <col min="21" max="21" width="9.1796875" style="1"/>
     <col min="22" max="22" width="9.1796875" style="25"/>
-    <col min="23" max="23" width="9.1796875" style="1"/>
-    <col min="24" max="24" width="9.1796875" style="25"/>
-    <col min="25" max="16384" width="9.1796875" style="1"/>
+    <col min="23" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
@@ -1751,7 +3224,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>250</v>
@@ -1766,114 +3239,143 @@
         <v>259</v>
       </c>
       <c r="H2" s="26" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="I2" s="26" t="s">
         <v>260</v>
       </c>
+      <c r="J2" s="26" t="s">
+        <v>253</v>
+      </c>
       <c r="K2" s="26" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="L2" s="26" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="M2" s="26" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="N2" s="26" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="O2" s="26" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="P2" s="26" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="Q2" s="26" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="R2" s="26" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="S2" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="T2" s="26" t="s">
+        <v>266</v>
+      </c>
+      <c r="U2" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="T2" s="26" t="s">
+      <c r="V2" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="W2" s="26" t="s">
         <v>268</v>
       </c>
-      <c r="U2" s="26" t="s">
+      <c r="X2" s="26" t="s">
         <v>269</v>
       </c>
-      <c r="V2" s="26" t="s">
+      <c r="Y2" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="W2" s="26" t="s">
+      <c r="Z2" s="26" t="s">
         <v>271</v>
       </c>
-      <c r="X2" s="26" t="s">
-        <v>252</v>
-      </c>
-      <c r="Y2" s="26" t="s">
+      <c r="AA2" s="26" t="s">
         <v>272</v>
       </c>
-      <c r="Z2" s="26" t="s">
+      <c r="AB2" s="26" t="s">
         <v>273</v>
       </c>
-      <c r="AA2" s="26" t="s">
+    </row>
+    <row r="3" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="34">
+        <v>271483</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>275</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3" s="35" t="s">
+        <v>276</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>277</v>
+      </c>
+      <c r="G3" s="37">
+        <v>7.7</v>
+      </c>
+      <c r="H3" s="38" t="str">
+        <f t="shared" ref="H3" si="0">IF(G3&lt;250, "&lt;250M", "&gt;=250M")</f>
+        <v>&lt;250M</v>
+      </c>
+      <c r="I3" s="39" t="str">
+        <f>_xlfn.XLOOKUP(A3,'[1]FY24 WLA'!$A:$A,'[1]FY24 WLA'!$AD:$AD)</f>
+        <v>EN</v>
+      </c>
+      <c r="J3" s="40" t="s">
+        <v>278</v>
+      </c>
+      <c r="K3" s="41" t="s">
+        <v>279</v>
+      </c>
+      <c r="L3" s="40" t="s">
+        <v>278</v>
+      </c>
+      <c r="M3" s="41" t="s">
+        <v>280</v>
+      </c>
+      <c r="N3" s="40" t="s">
+        <v>281</v>
+      </c>
+      <c r="O3" s="41" t="s">
+        <v>282</v>
+      </c>
+      <c r="P3" s="37" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q3"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="V3" s="37"/>
+      <c r="W3" s="37"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="42"/>
+      <c r="Z3" s="42" t="s">
+        <v>284</v>
+      </c>
+      <c r="AD3" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="AB2" s="26" t="s">
-        <v>275</v>
-      </c>
-      <c r="AC2" s="26" t="s">
-        <v>276</v>
-      </c>
-      <c r="AD2" s="26" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>278</v>
-      </c>
-      <c r="B3" t="s">
-        <v>279</v>
-      </c>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3" t="s">
-        <v>261</v>
-      </c>
-      <c r="F3" t="s">
-        <v>262</v>
-      </c>
-      <c r="G3">
-        <v>49.02</v>
-      </c>
-      <c r="H3"/>
-      <c r="I3" t="s">
-        <v>264</v>
-      </c>
-      <c r="K3" t="s">
-        <v>264</v>
-      </c>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3"/>
-      <c r="O3"/>
-      <c r="P3"/>
-      <c r="Q3"/>
-      <c r="R3"/>
-      <c r="S3"/>
-      <c r="X3" t="s">
-        <v>263</v>
-      </c>
-      <c r="AF3" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3 M3 O3" xr:uid="{C67EE4E1-D3B1-446A-A902-2B6DE67CE992}">
+      <formula1>INDIRECT(J3)</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>